<commit_message>
Removed Email and added download PDF report
</commit_message>
<xml_diff>
--- a/src/data/Money Survey V1.0 - Data for App.xlsx
+++ b/src/data/Money Survey V1.0 - Data for App.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\financial-wellbeing-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7680A0-B596-4447-94B4-FBA774DFF442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0E1BB1-A216-471F-A716-4BF9820FB4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2865" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome" sheetId="5" r:id="rId1"/>
     <sheet name="Themes" sheetId="4" r:id="rId2"/>
     <sheet name="Money Questions" sheetId="3" r:id="rId3"/>
-    <sheet name="Motivation" sheetId="6" r:id="rId4"/>
+    <sheet name="EmailKeys" sheetId="7" r:id="rId4"/>
+    <sheet name="Motivation" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Money Questions'!$B$1:$F$7</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="142">
   <si>
     <t>How good are you at money? Let's find out by answering some questions…</t>
   </si>
@@ -462,6 +463,12 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>RESEND API Key</t>
+  </si>
+  <si>
+    <t>re_J8BPpLQT_8eTYwn5ZstWPxgGxCYeLbA7a</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A68A07C-A95D-0B45-B4E1-0FBF27F98BB9}">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -2847,6 +2854,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCB3EEF-6DC6-4B33-BAC3-106D6E5EE2A4}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0A8E34-6EDA-4FBC-95D6-C915587DA356}">
   <dimension ref="B1:J32"/>
   <sheetViews>

</xml_diff>